<commit_message>
Minor changes with xpath
</commit_message>
<xml_diff>
--- a/src/test/resources/Policy.xlsx
+++ b/src/test/resources/Policy.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>₹798/month</t>
   </si>
@@ -41,6 +41,33 @@
   </si>
   <si>
     <t>₹797/month</t>
+  </si>
+  <si>
+    <t>Reliance</t>
+  </si>
+  <si>
+    <t>Student Silver</t>
+  </si>
+  <si>
+    <t>₹2,788</t>
+  </si>
+  <si>
+    <t>Bajaj Allianz</t>
+  </si>
+  <si>
+    <t>Student Elite</t>
+  </si>
+  <si>
+    <t>₹2,874</t>
+  </si>
+  <si>
+    <t>Care Health</t>
+  </si>
+  <si>
+    <t>Student Explore Plus</t>
+  </si>
+  <si>
+    <t>₹3,484</t>
   </si>
 </sst>
 </file>
@@ -359,14 +386,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>